<commit_message>
bảng lương bảo hiểm
</commit_message>
<xml_diff>
--- a/it_api/wwwroot/report/excel/Bảng lương.xlsx
+++ b/it_api/wwwroot/report/excel/Bảng lương.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\netcore\it_api\it_api\wwwroot\report\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE355D52-792D-4864-B594-A7FCAB35E185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3396BF92-A5B5-4CF8-876B-BC268282CD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tất cả" sheetId="18" r:id="rId1"/>
@@ -816,6 +816,81 @@
     <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -828,88 +903,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="15" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="15" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="25" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2392,11 +2392,11 @@
   </sheetPr>
   <dimension ref="A1:AM29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="C25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,11 +2417,12 @@
     <col min="14" max="14" width="16.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="3" customWidth="1"/>
     <col min="19" max="19" width="8.5703125" style="3" customWidth="1"/>
     <col min="20" max="20" width="11.140625" style="4" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="3" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="14.140625" style="3" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="3" hidden="1" customWidth="1"/>
@@ -2432,8 +2433,8 @@
     <col min="30" max="30" width="14.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="31" max="32" width="12.42578125" style="3" customWidth="1"/>
     <col min="33" max="33" width="12.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="3" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="3" customWidth="1"/>
     <col min="36" max="36" width="13.85546875" style="3" customWidth="1"/>
     <col min="37" max="37" width="7.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="0" style="3" hidden="1" customWidth="1"/>
@@ -2495,17 +2496,17 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="117" t="s">
+      <c r="P5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="10"/>
@@ -2534,17 +2535,17 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-      <c r="P6" s="118" t="s">
+      <c r="P6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="118"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="118"/>
-      <c r="X6" s="118"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="13"/>
@@ -2567,8 +2568,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -2598,110 +2599,110 @@
     </row>
     <row r="8" spans="1:39" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="112" t="s">
+      <c r="A9" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="123" t="s">
+      <c r="G9" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="97" t="s">
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="124" t="s">
+      <c r="R9" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="97" t="s">
+      <c r="S9" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="100" t="s">
+      <c r="T9" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="124" t="s">
+      <c r="U9" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="123" t="s">
+      <c r="V9" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="109" t="s">
+      <c r="W9" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="110"/>
-      <c r="Y9" s="97" t="s">
+      <c r="X9" s="113"/>
+      <c r="Y9" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="102" t="s">
+      <c r="Z9" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="AA9" s="102"/>
-      <c r="AB9" s="102"/>
-      <c r="AC9" s="103" t="s">
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AD9" s="97" t="s">
+      <c r="AD9" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="AE9" s="106" t="s">
+      <c r="AE9" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AF9" s="106" t="s">
+      <c r="AF9" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="AG9" s="106" t="s">
+      <c r="AG9" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="AH9" s="112" t="s">
+      <c r="AH9" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="AI9" s="113" t="s">
+      <c r="AI9" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="AJ9" s="97" t="s">
+      <c r="AJ9" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="AK9" s="115" t="s">
+      <c r="AK9" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="AL9" s="95" t="s">
+      <c r="AL9" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="AM9" s="108" t="s">
+      <c r="AM9" s="111" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="97"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="21" t="s">
         <v>45</v>
       </c>
@@ -2729,19 +2730,19 @@
       <c r="P10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="101"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="97"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="123"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="102"/>
       <c r="W10" s="21" t="s">
         <v>28</v>
       </c>
       <c r="X10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="99"/>
+      <c r="Y10" s="104"/>
       <c r="Z10" s="23" t="s">
         <v>30</v>
       </c>
@@ -2751,24 +2752,24 @@
       <c r="AB10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" s="103"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="107"/>
-      <c r="AF10" s="111"/>
-      <c r="AG10" s="107"/>
-      <c r="AH10" s="99"/>
-      <c r="AI10" s="114"/>
-      <c r="AJ10" s="98"/>
-      <c r="AK10" s="115"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="108"/>
+      <c r="AC10" s="124"/>
+      <c r="AD10" s="104"/>
+      <c r="AE10" s="110"/>
+      <c r="AF10" s="114"/>
+      <c r="AG10" s="110"/>
+      <c r="AH10" s="104"/>
+      <c r="AI10" s="116"/>
+      <c r="AJ10" s="103"/>
+      <c r="AK10" s="117"/>
+      <c r="AL10" s="121"/>
+      <c r="AM10" s="111"/>
     </row>
     <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
       <c r="F11" s="37"/>
@@ -3159,16 +3160,22 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="P15" s="39">
-        <f t="shared" ref="P15" si="4">SUMIF($E11:$E14,"",P11:P14)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q15" s="39">
-        <f ca="1">SUMIF($E11:$E14,"",Q11:Q13)</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="39"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="S15" s="39">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -3210,11 +3217,11 @@
         <v>0</v>
       </c>
       <c r="AC15" s="39">
-        <f t="shared" ref="AC15" si="5">SUMIF($E11:$E14,"",AC11:AC14)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD15" s="39" t="e">
-        <f>SUMIF($E11:$E14,"",AD11:AD14)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE15" s="39" t="e">
@@ -3331,24 +3338,24 @@
     </row>
     <row r="18" spans="1:39" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="46"/>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="93"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
       <c r="K18" s="48"/>
-      <c r="R18" s="94" t="s">
+      <c r="R18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="S18" s="94"/>
-      <c r="T18" s="94"/>
-      <c r="U18" s="94"/>
-      <c r="W18" s="94" t="s">
+      <c r="S18" s="119"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="119"/>
+      <c r="W18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="X18" s="94"/>
-      <c r="Y18" s="94"/>
+      <c r="X18" s="119"/>
+      <c r="Y18" s="119"/>
       <c r="AA18" s="49"/>
       <c r="AB18" s="50"/>
       <c r="AE18" s="51"/>
@@ -3363,24 +3370,24 @@
       <c r="AM18" s="52"/>
     </row>
     <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="116" t="s">
+      <c r="F19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="116"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="K19" s="54"/>
-      <c r="R19" s="116" t="s">
+      <c r="R19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="S19" s="116"/>
-      <c r="T19" s="116"/>
-      <c r="U19" s="116"/>
-      <c r="W19" s="116" t="s">
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="W19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="116"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
       <c r="AC19" s="44"/>
       <c r="AE19" s="42"/>
       <c r="AF19" s="42"/>
@@ -3602,6 +3609,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="AL9:AL10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="H9:P9"/>
+    <mergeCell ref="AC9:AC10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="AG9:AG10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="AF9:AF10"/>
+    <mergeCell ref="AH9:AH10"/>
+    <mergeCell ref="AI9:AI10"/>
+    <mergeCell ref="AJ9:AJ10"/>
+    <mergeCell ref="AK9:AK10"/>
     <mergeCell ref="R19:U19"/>
     <mergeCell ref="P5:X5"/>
     <mergeCell ref="P6:X6"/>
@@ -3618,28 +3647,6 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="W19:Y19"/>
     <mergeCell ref="U9:U10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="AG9:AG10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
-    <mergeCell ref="AF9:AF10"/>
-    <mergeCell ref="AH9:AH10"/>
-    <mergeCell ref="AI9:AI10"/>
-    <mergeCell ref="AJ9:AJ10"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="AL9:AL10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="H9:P9"/>
-    <mergeCell ref="AC9:AC10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.17" right="0" top="0" bottom="0.2" header="0.2" footer="0.21"/>
@@ -3664,7 +3671,7 @@
       <pane xSplit="3" ySplit="11" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3685,11 +3692,12 @@
     <col min="14" max="14" width="16.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="3" customWidth="1"/>
     <col min="19" max="19" width="8.5703125" style="3" customWidth="1"/>
     <col min="20" max="20" width="11.140625" style="4" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="3" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="14.140625" style="3" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="3" hidden="1" customWidth="1"/>
@@ -3700,8 +3708,8 @@
     <col min="30" max="30" width="14.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="31" max="32" width="12.42578125" style="3" customWidth="1"/>
     <col min="33" max="33" width="12.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="3" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="3" customWidth="1"/>
     <col min="36" max="36" width="13.85546875" style="3" customWidth="1"/>
     <col min="37" max="37" width="7.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="0" style="3" hidden="1" customWidth="1"/>
@@ -3763,17 +3771,17 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="117" t="s">
+      <c r="P5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="10"/>
@@ -3802,17 +3810,17 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-      <c r="P6" s="118" t="s">
+      <c r="P6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="118"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="118"/>
-      <c r="X6" s="118"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="13"/>
@@ -3835,8 +3843,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -3866,110 +3874,110 @@
     </row>
     <row r="8" spans="1:39" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="112" t="s">
+      <c r="A9" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="123" t="s">
+      <c r="G9" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="97" t="s">
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="124" t="s">
+      <c r="R9" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="97" t="s">
+      <c r="S9" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="100" t="s">
+      <c r="T9" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="124" t="s">
+      <c r="U9" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="123" t="s">
+      <c r="V9" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="109" t="s">
+      <c r="W9" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="110"/>
-      <c r="Y9" s="97" t="s">
+      <c r="X9" s="113"/>
+      <c r="Y9" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="102" t="s">
+      <c r="Z9" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="AA9" s="102"/>
-      <c r="AB9" s="102"/>
-      <c r="AC9" s="103" t="s">
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AD9" s="97" t="s">
+      <c r="AD9" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="AE9" s="106" t="s">
+      <c r="AE9" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AF9" s="106" t="s">
+      <c r="AF9" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="AG9" s="106" t="s">
+      <c r="AG9" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="AH9" s="112" t="s">
+      <c r="AH9" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="AI9" s="113" t="s">
+      <c r="AI9" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="AJ9" s="97" t="s">
+      <c r="AJ9" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="AK9" s="115" t="s">
+      <c r="AK9" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="AL9" s="95" t="s">
+      <c r="AL9" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="AM9" s="108" t="s">
+      <c r="AM9" s="111" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="97"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="21" t="s">
         <v>45</v>
       </c>
@@ -3997,19 +4005,19 @@
       <c r="P10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="101"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="97"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="123"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="102"/>
       <c r="W10" s="21" t="s">
         <v>28</v>
       </c>
       <c r="X10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="99"/>
+      <c r="Y10" s="104"/>
       <c r="Z10" s="23" t="s">
         <v>30</v>
       </c>
@@ -4019,24 +4027,24 @@
       <c r="AB10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" s="103"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="107"/>
-      <c r="AF10" s="111"/>
-      <c r="AG10" s="107"/>
-      <c r="AH10" s="99"/>
-      <c r="AI10" s="114"/>
-      <c r="AJ10" s="98"/>
-      <c r="AK10" s="115"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="108"/>
+      <c r="AC10" s="124"/>
+      <c r="AD10" s="104"/>
+      <c r="AE10" s="110"/>
+      <c r="AF10" s="114"/>
+      <c r="AG10" s="110"/>
+      <c r="AH10" s="104"/>
+      <c r="AI10" s="116"/>
+      <c r="AJ10" s="103"/>
+      <c r="AK10" s="117"/>
+      <c r="AL10" s="121"/>
+      <c r="AM10" s="111"/>
     </row>
     <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
       <c r="F11" s="37"/>
@@ -4427,16 +4435,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="P15" s="39">
-        <f t="shared" ref="P15" si="3">SUMIF($E11:$E14,"",P11:P14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q15" s="39">
-        <f ca="1">SUMIF($E11:$E14,"",Q11:Q13)</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="39"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S15" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -4482,7 +4496,7 @@
         <v>0</v>
       </c>
       <c r="AD15" s="39" t="e">
-        <f>SUMIF($E11:$E14,"",AD11:AD14)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE15" s="39" t="e">
@@ -4599,24 +4613,24 @@
     </row>
     <row r="18" spans="1:39" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="46"/>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="93"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
       <c r="K18" s="48"/>
-      <c r="R18" s="94" t="s">
+      <c r="R18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="S18" s="94"/>
-      <c r="T18" s="94"/>
-      <c r="U18" s="94"/>
-      <c r="W18" s="94" t="s">
+      <c r="S18" s="119"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="119"/>
+      <c r="W18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="X18" s="94"/>
-      <c r="Y18" s="94"/>
+      <c r="X18" s="119"/>
+      <c r="Y18" s="119"/>
       <c r="AA18" s="49"/>
       <c r="AB18" s="50"/>
       <c r="AE18" s="51"/>
@@ -4631,24 +4645,24 @@
       <c r="AM18" s="52"/>
     </row>
     <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="116" t="s">
+      <c r="F19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="116"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="K19" s="54"/>
-      <c r="R19" s="116" t="s">
+      <c r="R19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="S19" s="116"/>
-      <c r="T19" s="116"/>
-      <c r="U19" s="116"/>
-      <c r="W19" s="116" t="s">
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="W19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="116"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
       <c r="AC19" s="44"/>
       <c r="AE19" s="42"/>
       <c r="AF19" s="42"/>
@@ -4870,25 +4884,11 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Z9:AB9"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:P9"/>
-    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="R19:U19"/>
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="AE9:AE10"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="AL9:AL10"/>
     <mergeCell ref="AK9:AK10"/>
@@ -4902,12 +4902,26 @@
     <mergeCell ref="Q9:Q10"/>
     <mergeCell ref="R9:R10"/>
     <mergeCell ref="S9:S10"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:P9"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="R19:U19"/>
-    <mergeCell ref="W19:Y19"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="AE9:AE10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="Y9:Y10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.17" right="0" top="0" bottom="0.2" header="0.2" footer="0.21"/>
@@ -4929,7 +4943,7 @@
       <pane xSplit="3" ySplit="11" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4950,11 +4964,12 @@
     <col min="14" max="14" width="16.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="3" customWidth="1"/>
     <col min="19" max="19" width="8.5703125" style="3" customWidth="1"/>
     <col min="20" max="20" width="11.140625" style="4" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="3" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="14.140625" style="3" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="3" hidden="1" customWidth="1"/>
@@ -4965,8 +4980,8 @@
     <col min="30" max="30" width="14.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="31" max="32" width="12.42578125" style="3" customWidth="1"/>
     <col min="33" max="33" width="12.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="3" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="3" customWidth="1"/>
     <col min="36" max="36" width="13.85546875" style="3" customWidth="1"/>
     <col min="37" max="37" width="7.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="0" style="3" hidden="1" customWidth="1"/>
@@ -5028,17 +5043,17 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="117" t="s">
+      <c r="P5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="10"/>
@@ -5067,17 +5082,17 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-      <c r="P6" s="118" t="s">
+      <c r="P6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="118"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="118"/>
-      <c r="X6" s="118"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="13"/>
@@ -5100,8 +5115,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -5131,110 +5146,110 @@
     </row>
     <row r="8" spans="1:39" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="112" t="s">
+      <c r="A9" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="123" t="s">
+      <c r="G9" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="97" t="s">
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="124" t="s">
+      <c r="R9" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="97" t="s">
+      <c r="S9" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="100" t="s">
+      <c r="T9" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="124" t="s">
+      <c r="U9" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="123" t="s">
+      <c r="V9" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="109" t="s">
+      <c r="W9" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="110"/>
-      <c r="Y9" s="97" t="s">
+      <c r="X9" s="113"/>
+      <c r="Y9" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="102" t="s">
+      <c r="Z9" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="AA9" s="102"/>
-      <c r="AB9" s="102"/>
-      <c r="AC9" s="103" t="s">
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AD9" s="97" t="s">
+      <c r="AD9" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="AE9" s="106" t="s">
+      <c r="AE9" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AF9" s="106" t="s">
+      <c r="AF9" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="AG9" s="106" t="s">
+      <c r="AG9" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="AH9" s="112" t="s">
+      <c r="AH9" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="AI9" s="113" t="s">
+      <c r="AI9" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="AJ9" s="97" t="s">
+      <c r="AJ9" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="AK9" s="115" t="s">
+      <c r="AK9" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="AL9" s="95" t="s">
+      <c r="AL9" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="AM9" s="108" t="s">
+      <c r="AM9" s="111" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="97"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="21" t="s">
         <v>45</v>
       </c>
@@ -5262,19 +5277,19 @@
       <c r="P10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="101"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="97"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="123"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="102"/>
       <c r="W10" s="21" t="s">
         <v>28</v>
       </c>
       <c r="X10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="99"/>
+      <c r="Y10" s="104"/>
       <c r="Z10" s="23" t="s">
         <v>30</v>
       </c>
@@ -5284,24 +5299,24 @@
       <c r="AB10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" s="103"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="107"/>
-      <c r="AF10" s="111"/>
-      <c r="AG10" s="107"/>
-      <c r="AH10" s="99"/>
-      <c r="AI10" s="114"/>
-      <c r="AJ10" s="98"/>
-      <c r="AK10" s="115"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="108"/>
+      <c r="AC10" s="124"/>
+      <c r="AD10" s="104"/>
+      <c r="AE10" s="110"/>
+      <c r="AF10" s="114"/>
+      <c r="AG10" s="110"/>
+      <c r="AH10" s="104"/>
+      <c r="AI10" s="116"/>
+      <c r="AJ10" s="103"/>
+      <c r="AK10" s="117"/>
+      <c r="AL10" s="121"/>
+      <c r="AM10" s="111"/>
     </row>
     <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
       <c r="F11" s="37"/>
@@ -5692,16 +5707,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="P15" s="39">
-        <f t="shared" ref="P15" si="3">SUMIF($E11:$E14,"",P11:P14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q15" s="39">
-        <f ca="1">SUMIF($E11:$E14,"",Q11:Q13)</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="39"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S15" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -5747,7 +5768,7 @@
         <v>0</v>
       </c>
       <c r="AD15" s="39" t="e">
-        <f>SUMIF($E11:$E14,"",AD11:AD14)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE15" s="39" t="e">
@@ -5864,24 +5885,24 @@
     </row>
     <row r="18" spans="1:39" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="46"/>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="93"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
       <c r="K18" s="48"/>
-      <c r="R18" s="94" t="s">
+      <c r="R18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="S18" s="94"/>
-      <c r="T18" s="94"/>
-      <c r="U18" s="94"/>
-      <c r="W18" s="94" t="s">
+      <c r="S18" s="119"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="119"/>
+      <c r="W18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="X18" s="94"/>
-      <c r="Y18" s="94"/>
+      <c r="X18" s="119"/>
+      <c r="Y18" s="119"/>
       <c r="AA18" s="49"/>
       <c r="AB18" s="50"/>
       <c r="AE18" s="51"/>
@@ -5896,24 +5917,24 @@
       <c r="AM18" s="52"/>
     </row>
     <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="116" t="s">
+      <c r="F19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="116"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="K19" s="54"/>
-      <c r="R19" s="116" t="s">
+      <c r="R19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="S19" s="116"/>
-      <c r="T19" s="116"/>
-      <c r="U19" s="116"/>
-      <c r="W19" s="116" t="s">
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="W19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="116"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
       <c r="AC19" s="44"/>
       <c r="AE19" s="42"/>
       <c r="AF19" s="42"/>
@@ -6135,17 +6156,19 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:P9"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="R19:U19"/>
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="AL9:AL10"/>
     <mergeCell ref="AK9:AK10"/>
@@ -6158,21 +6181,19 @@
     <mergeCell ref="AF9:AF10"/>
     <mergeCell ref="AC9:AC10"/>
     <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:P9"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="R19:U19"/>
-    <mergeCell ref="W19:Y19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6182,11 +6203,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97666D5E-E27B-4C7D-8F3C-37539DDADFBC}">
   <dimension ref="A1:AM29"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane xSplit="3" ySplit="11" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6207,11 +6228,12 @@
     <col min="14" max="14" width="16.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="3" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15" style="3" customWidth="1"/>
-    <col min="17" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="16" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="3" customWidth="1"/>
     <col min="19" max="19" width="8.5703125" style="3" customWidth="1"/>
     <col min="20" max="20" width="11.140625" style="4" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="3" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="14.140625" style="3" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="10.140625" style="3" hidden="1" customWidth="1"/>
@@ -6222,8 +6244,8 @@
     <col min="30" max="30" width="14.7109375" style="3" hidden="1" customWidth="1"/>
     <col min="31" max="32" width="12.42578125" style="3" customWidth="1"/>
     <col min="33" max="33" width="12.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="15" style="3" customWidth="1"/>
-    <col min="35" max="35" width="15.28515625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="3" customWidth="1"/>
     <col min="36" max="36" width="13.85546875" style="3" customWidth="1"/>
     <col min="37" max="37" width="7.85546875" style="3" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="0" style="3" hidden="1" customWidth="1"/>
@@ -6285,17 +6307,17 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
-      <c r="P5" s="117" t="s">
+      <c r="P5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="117"/>
-      <c r="R5" s="117"/>
-      <c r="S5" s="117"/>
-      <c r="T5" s="117"/>
-      <c r="U5" s="117"/>
-      <c r="V5" s="117"/>
-      <c r="W5" s="117"/>
-      <c r="X5" s="117"/>
+      <c r="Q5" s="94"/>
+      <c r="R5" s="94"/>
+      <c r="S5" s="94"/>
+      <c r="T5" s="94"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="10"/>
@@ -6324,17 +6346,17 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
-      <c r="P6" s="118" t="s">
+      <c r="P6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="118"/>
-      <c r="R6" s="118"/>
-      <c r="S6" s="118"/>
-      <c r="T6" s="118"/>
-      <c r="U6" s="118"/>
-      <c r="V6" s="118"/>
-      <c r="W6" s="118"/>
-      <c r="X6" s="118"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
+      <c r="S6" s="95"/>
+      <c r="T6" s="95"/>
+      <c r="U6" s="95"/>
+      <c r="V6" s="95"/>
+      <c r="W6" s="95"/>
+      <c r="X6" s="95"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="13"/>
@@ -6357,8 +6379,8 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -6388,110 +6410,110 @@
     </row>
     <row r="8" spans="1:39" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:39" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="112" t="s">
+      <c r="A9" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="123" t="s">
+      <c r="G9" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="102"/>
-      <c r="L9" s="102"/>
-      <c r="M9" s="102"/>
-      <c r="N9" s="102"/>
-      <c r="O9" s="102"/>
-      <c r="P9" s="102"/>
-      <c r="Q9" s="97" t="s">
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="R9" s="124" t="s">
+      <c r="R9" s="106" t="s">
         <v>15</v>
       </c>
-      <c r="S9" s="97" t="s">
+      <c r="S9" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="100" t="s">
+      <c r="T9" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="124" t="s">
+      <c r="U9" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="V9" s="123" t="s">
+      <c r="V9" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="109" t="s">
+      <c r="W9" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="X9" s="110"/>
-      <c r="Y9" s="97" t="s">
+      <c r="X9" s="113"/>
+      <c r="Y9" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="Z9" s="102" t="s">
+      <c r="Z9" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="AA9" s="102"/>
-      <c r="AB9" s="102"/>
-      <c r="AC9" s="103" t="s">
+      <c r="AA9" s="97"/>
+      <c r="AB9" s="97"/>
+      <c r="AC9" s="124" t="s">
         <v>48</v>
       </c>
-      <c r="AD9" s="97" t="s">
+      <c r="AD9" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="AE9" s="106" t="s">
+      <c r="AE9" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="AF9" s="106" t="s">
+      <c r="AF9" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="AG9" s="106" t="s">
+      <c r="AG9" s="109" t="s">
         <v>37</v>
       </c>
-      <c r="AH9" s="112" t="s">
+      <c r="AH9" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="AI9" s="113" t="s">
+      <c r="AI9" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="AJ9" s="97" t="s">
+      <c r="AJ9" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="AK9" s="115" t="s">
+      <c r="AK9" s="117" t="s">
         <v>25</v>
       </c>
-      <c r="AL9" s="95" t="s">
+      <c r="AL9" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="AM9" s="108" t="s">
+      <c r="AM9" s="111" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:39" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="120"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="97"/>
+      <c r="A10" s="98"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="102"/>
       <c r="H10" s="21" t="s">
         <v>45</v>
       </c>
@@ -6519,19 +6541,19 @@
       <c r="P10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="99"/>
-      <c r="T10" s="101"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="97"/>
+      <c r="Q10" s="103"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="123"/>
+      <c r="U10" s="106"/>
+      <c r="V10" s="102"/>
       <c r="W10" s="21" t="s">
         <v>28</v>
       </c>
       <c r="X10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Y10" s="99"/>
+      <c r="Y10" s="104"/>
       <c r="Z10" s="23" t="s">
         <v>30</v>
       </c>
@@ -6541,24 +6563,24 @@
       <c r="AB10" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AC10" s="103"/>
-      <c r="AD10" s="99"/>
-      <c r="AE10" s="107"/>
-      <c r="AF10" s="111"/>
-      <c r="AG10" s="107"/>
-      <c r="AH10" s="99"/>
-      <c r="AI10" s="114"/>
-      <c r="AJ10" s="98"/>
-      <c r="AK10" s="115"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="108"/>
+      <c r="AC10" s="124"/>
+      <c r="AD10" s="104"/>
+      <c r="AE10" s="110"/>
+      <c r="AF10" s="114"/>
+      <c r="AG10" s="110"/>
+      <c r="AH10" s="104"/>
+      <c r="AI10" s="116"/>
+      <c r="AJ10" s="103"/>
+      <c r="AK10" s="117"/>
+      <c r="AL10" s="121"/>
+      <c r="AM10" s="111"/>
     </row>
     <row r="11" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="105"/>
-      <c r="C11" s="105"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
       <c r="F11" s="37"/>
@@ -6949,16 +6971,22 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="P15" s="39">
-        <f t="shared" ref="P15" si="3">SUMIF($E11:$E14,"",P11:P14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q15" s="39">
-        <f ca="1">SUMIF($E11:$E14,"",Q11:Q13)</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="39"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="S15" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -7004,7 +7032,7 @@
         <v>0</v>
       </c>
       <c r="AD15" s="39" t="e">
-        <f>SUMIF($E11:$E14,"",AD11:AD14)</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE15" s="39" t="e">
@@ -7121,24 +7149,24 @@
     </row>
     <row r="18" spans="1:39" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="46"/>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="93"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="47"/>
       <c r="I18" s="47"/>
       <c r="K18" s="48"/>
-      <c r="R18" s="94" t="s">
+      <c r="R18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="S18" s="94"/>
-      <c r="T18" s="94"/>
-      <c r="U18" s="94"/>
-      <c r="W18" s="94" t="s">
+      <c r="S18" s="119"/>
+      <c r="T18" s="119"/>
+      <c r="U18" s="119"/>
+      <c r="W18" s="119" t="s">
         <v>33</v>
       </c>
-      <c r="X18" s="94"/>
-      <c r="Y18" s="94"/>
+      <c r="X18" s="119"/>
+      <c r="Y18" s="119"/>
       <c r="AA18" s="49"/>
       <c r="AB18" s="50"/>
       <c r="AE18" s="51"/>
@@ -7153,24 +7181,24 @@
       <c r="AM18" s="52"/>
     </row>
     <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="116" t="s">
+      <c r="F19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="116"/>
+      <c r="G19" s="93"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="K19" s="54"/>
-      <c r="R19" s="116" t="s">
+      <c r="R19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="S19" s="116"/>
-      <c r="T19" s="116"/>
-      <c r="U19" s="116"/>
-      <c r="W19" s="116" t="s">
+      <c r="S19" s="93"/>
+      <c r="T19" s="93"/>
+      <c r="U19" s="93"/>
+      <c r="W19" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="X19" s="116"/>
-      <c r="Y19" s="116"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
       <c r="AC19" s="44"/>
       <c r="AE19" s="42"/>
       <c r="AF19" s="42"/>
@@ -7392,17 +7420,19 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H9:P9"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="AM9:AM10"/>
+    <mergeCell ref="R19:U19"/>
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="P5:X5"/>
+    <mergeCell ref="P6:X6"/>
+    <mergeCell ref="V9:V10"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="S9:S10"/>
+    <mergeCell ref="T9:T10"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="AL9:AL10"/>
     <mergeCell ref="AK9:AK10"/>
@@ -7415,21 +7445,19 @@
     <mergeCell ref="AF9:AF10"/>
     <mergeCell ref="AC9:AC10"/>
     <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H9:P9"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
-    <mergeCell ref="P5:X5"/>
-    <mergeCell ref="P6:X6"/>
-    <mergeCell ref="V9:V10"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="Y9:Y10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="S9:S10"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="AM9:AM10"/>
-    <mergeCell ref="R19:U19"/>
-    <mergeCell ref="W19:Y19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>